<commit_message>
Updated Meck-Pom. Also changed abs_ == 0 to NA and created indicator to show where this was the case.
</commit_message>
<xml_diff>
--- a/data/municipal_elections/raw_data/mecklenburg_vorpommern/mecklenburg_vorpommern_landtagswahlen_2019.xlsx
+++ b/data/municipal_elections/raw_data/mecklenburg_vorpommern/mecklenburg_vorpommern_landtagswahlen_2019.xlsx
@@ -5,22 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flosic/Documents/GitHub/german_election_data/data/municipal_elections/raw_data/mecklenburg_vorpommern/new processed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flosic/Documents/GitHub/german_election_data/data/municipal_elections/raw_data/mecklenburg_vorpommern/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4654B7D8-22DC-984C-BC9A-2B263D9F5EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18122373-F498-8745-9C70-F56D1752A4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="15960" windowHeight="14300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="15960" windowHeight="13360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - mecklenburg_vorpommer" sheetId="1" r:id="rId1"/>
+    <sheet name="summary" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>Ausgabe</t>
   </si>
@@ -185,17 +185,35 @@
   </si>
   <si>
     <t>Schwerin</t>
+  </si>
+  <si>
+    <t>Gemeindenummer</t>
+  </si>
+  <si>
+    <t>13003000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFE6E1DC"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -250,7 +268,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -268,6 +286,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1429,384 +1456,393 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AZ3"/>
+  <dimension ref="A1:BA3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="1" customWidth="1"/>
-    <col min="5" max="6" width="13.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="7" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.83203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7" style="1" customWidth="1"/>
-    <col min="14" max="14" width="7.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="7" style="1" customWidth="1"/>
-    <col min="16" max="17" width="6.1640625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="8.1640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="12.1640625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="5.1640625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="6.33203125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="5.83203125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="5.1640625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="13" style="1" customWidth="1"/>
-    <col min="25" max="25" width="9.33203125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="16.5" style="1" customWidth="1"/>
-    <col min="27" max="27" width="5.1640625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="30.33203125" style="1" customWidth="1"/>
-    <col min="29" max="29" width="5.1640625" style="1" customWidth="1"/>
-    <col min="30" max="30" width="4.83203125" style="1" customWidth="1"/>
-    <col min="31" max="31" width="5.1640625" style="1" customWidth="1"/>
-    <col min="32" max="32" width="13.5" style="1" customWidth="1"/>
-    <col min="33" max="33" width="16.1640625" style="1" customWidth="1"/>
-    <col min="34" max="34" width="16.5" style="1" customWidth="1"/>
-    <col min="35" max="35" width="15.1640625" style="1" customWidth="1"/>
-    <col min="36" max="36" width="16.1640625" style="1" customWidth="1"/>
-    <col min="37" max="37" width="4.5" style="1" customWidth="1"/>
-    <col min="38" max="38" width="5.1640625" style="1" customWidth="1"/>
-    <col min="39" max="39" width="6" style="1" customWidth="1"/>
-    <col min="40" max="40" width="6.1640625" style="1" customWidth="1"/>
-    <col min="41" max="41" width="10" style="1" customWidth="1"/>
-    <col min="42" max="42" width="13.33203125" style="1" customWidth="1"/>
-    <col min="43" max="43" width="8.1640625" style="1" customWidth="1"/>
-    <col min="44" max="45" width="6.1640625" style="1" customWidth="1"/>
-    <col min="46" max="46" width="13.5" style="1" customWidth="1"/>
-    <col min="47" max="47" width="5.83203125" style="1" customWidth="1"/>
-    <col min="48" max="48" width="5.33203125" style="1" customWidth="1"/>
-    <col min="49" max="49" width="6.1640625" style="1" customWidth="1"/>
-    <col min="50" max="50" width="18.6640625" style="1" customWidth="1"/>
-    <col min="51" max="51" width="5.1640625" style="1" customWidth="1"/>
-    <col min="52" max="52" width="12.83203125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="8.33203125" style="1" customWidth="1"/>
-    <col min="54" max="16384" width="8.33203125" style="1"/>
+    <col min="3" max="3" width="23" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="1" customWidth="1"/>
+    <col min="6" max="7" width="13.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="7" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="7" style="1" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="7" style="1" customWidth="1"/>
+    <col min="17" max="18" width="6.1640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="8.1640625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="12.1640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="5.1640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="6.33203125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="5.83203125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="5.1640625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="13" style="1" customWidth="1"/>
+    <col min="26" max="26" width="9.33203125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="16.5" style="1" customWidth="1"/>
+    <col min="28" max="28" width="5.1640625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="30.33203125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="5.1640625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="4.83203125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="5.1640625" style="1" customWidth="1"/>
+    <col min="33" max="33" width="13.5" style="1" customWidth="1"/>
+    <col min="34" max="34" width="16.1640625" style="1" customWidth="1"/>
+    <col min="35" max="35" width="16.5" style="1" customWidth="1"/>
+    <col min="36" max="36" width="15.1640625" style="1" customWidth="1"/>
+    <col min="37" max="37" width="16.1640625" style="1" customWidth="1"/>
+    <col min="38" max="38" width="4.5" style="1" customWidth="1"/>
+    <col min="39" max="39" width="5.1640625" style="1" customWidth="1"/>
+    <col min="40" max="40" width="6" style="1" customWidth="1"/>
+    <col min="41" max="41" width="6.1640625" style="1" customWidth="1"/>
+    <col min="42" max="42" width="10" style="1" customWidth="1"/>
+    <col min="43" max="43" width="13.33203125" style="1" customWidth="1"/>
+    <col min="44" max="44" width="8.1640625" style="1" customWidth="1"/>
+    <col min="45" max="46" width="6.1640625" style="1" customWidth="1"/>
+    <col min="47" max="47" width="13.5" style="1" customWidth="1"/>
+    <col min="48" max="48" width="5.83203125" style="1" customWidth="1"/>
+    <col min="49" max="49" width="5.33203125" style="1" customWidth="1"/>
+    <col min="50" max="50" width="6.1640625" style="1" customWidth="1"/>
+    <col min="51" max="51" width="18.6640625" style="1" customWidth="1"/>
+    <col min="52" max="52" width="5.1640625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="12.83203125" style="1" customWidth="1"/>
+    <col min="54" max="54" width="8.33203125" style="1" customWidth="1"/>
+    <col min="55" max="16384" width="8.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AT1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AU1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AV1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="3" t="s">
+      <c r="AW1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="3" t="s">
+      <c r="AX1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="3" t="s">
+      <c r="AY1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="3" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="3" t="s">
+      <c r="BA1" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:52" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B2" s="4">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="D2" s="4">
-        <v>162</v>
       </c>
       <c r="E2" s="4">
         <v>162</v>
       </c>
       <c r="F2" s="4">
+        <v>162</v>
+      </c>
+      <c r="G2" s="4">
         <v>173650</v>
       </c>
-      <c r="G2" s="4">
+      <c r="H2" s="4">
         <v>102304</v>
       </c>
-      <c r="H2" s="4">
+      <c r="I2" s="4">
         <v>58.9</v>
       </c>
-      <c r="I2" s="4">
+      <c r="J2" s="4">
         <v>4179</v>
       </c>
-      <c r="J2" s="4">
+      <c r="K2" s="4">
         <v>293275</v>
       </c>
-      <c r="K2" s="4">
+      <c r="L2" s="4">
         <v>42422</v>
       </c>
-      <c r="L2" s="4">
+      <c r="M2" s="4">
         <v>58405</v>
       </c>
-      <c r="M2" s="4">
+      <c r="N2" s="4">
         <v>42269</v>
       </c>
-      <c r="N2" s="4">
+      <c r="O2" s="4">
         <v>55616</v>
       </c>
-      <c r="O2" s="4">
+      <c r="P2" s="4">
         <v>28294</v>
       </c>
-      <c r="P2" s="4">
+      <c r="Q2" s="4">
         <v>9645</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="R2" s="4">
         <v>1633</v>
       </c>
-      <c r="R2" s="4">
+      <c r="S2" s="4">
         <v>1714</v>
       </c>
-      <c r="S2" s="5"/>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
       <c r="W2" s="5"/>
-      <c r="X2" s="4">
+      <c r="X2" s="5"/>
+      <c r="Y2" s="4">
         <v>2897</v>
       </c>
-      <c r="Y2" s="5"/>
       <c r="Z2" s="5"/>
       <c r="AA2" s="5"/>
       <c r="AB2" s="5"/>
       <c r="AC2" s="5"/>
       <c r="AD2" s="5"/>
       <c r="AE2" s="5"/>
-      <c r="AF2" s="4">
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="4">
         <v>3790</v>
       </c>
-      <c r="AG2" s="5"/>
       <c r="AH2" s="5"/>
       <c r="AI2" s="5"/>
       <c r="AJ2" s="5"/>
       <c r="AK2" s="5"/>
       <c r="AL2" s="5"/>
-      <c r="AM2" s="4">
+      <c r="AM2" s="5"/>
+      <c r="AN2" s="4">
         <v>1869</v>
       </c>
-      <c r="AN2" s="5"/>
-      <c r="AO2" s="4">
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="4">
         <v>7373</v>
       </c>
-      <c r="AP2" s="5"/>
       <c r="AQ2" s="5"/>
       <c r="AR2" s="5"/>
-      <c r="AS2" s="4">
+      <c r="AS2" s="5"/>
+      <c r="AT2" s="4">
         <v>21483</v>
       </c>
-      <c r="AT2" s="4">
+      <c r="AU2" s="4">
         <v>12086</v>
       </c>
-      <c r="AU2" s="5"/>
       <c r="AV2" s="5"/>
       <c r="AW2" s="5"/>
       <c r="AX2" s="5"/>
       <c r="AY2" s="5"/>
-      <c r="AZ2" s="4">
+      <c r="AZ2" s="5"/>
+      <c r="BA2" s="4">
         <v>3779</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:53" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B3" s="4">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="7">
+        <v>13004000</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="D3" s="4">
-        <v>71</v>
       </c>
       <c r="E3" s="4">
         <v>71</v>
       </c>
       <c r="F3" s="4">
+        <v>71</v>
+      </c>
+      <c r="G3" s="4">
         <v>78449</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>45526</v>
       </c>
-      <c r="H3" s="4">
+      <c r="I3" s="4">
         <v>58</v>
       </c>
-      <c r="I3" s="4">
+      <c r="J3" s="4">
         <v>1204</v>
       </c>
-      <c r="J3" s="4">
+      <c r="K3" s="4">
         <v>132816</v>
       </c>
-      <c r="K3" s="4">
+      <c r="L3" s="4">
         <v>22819</v>
       </c>
-      <c r="L3" s="4">
+      <c r="M3" s="4">
         <v>20601</v>
       </c>
-      <c r="M3" s="4">
+      <c r="N3" s="4">
         <v>22860</v>
       </c>
-      <c r="N3" s="4">
+      <c r="O3" s="4">
         <v>16064</v>
       </c>
-      <c r="O3" s="4">
+      <c r="P3" s="4">
         <v>20071</v>
       </c>
-      <c r="P3" s="4">
+      <c r="Q3" s="4">
         <v>5274</v>
       </c>
-      <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
-      <c r="S3" s="4">
+      <c r="S3" s="5"/>
+      <c r="T3" s="4">
         <v>1946</v>
       </c>
-      <c r="T3" s="5"/>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
       <c r="W3" s="5"/>
@@ -1827,22 +1863,23 @@
       <c r="AL3" s="5"/>
       <c r="AM3" s="5"/>
       <c r="AN3" s="5"/>
-      <c r="AO3" s="4">
+      <c r="AO3" s="5"/>
+      <c r="AP3" s="4">
         <v>4028</v>
       </c>
-      <c r="AP3" s="5"/>
       <c r="AQ3" s="5"/>
-      <c r="AR3" s="4">
+      <c r="AR3" s="5"/>
+      <c r="AS3" s="4">
         <v>18689</v>
       </c>
-      <c r="AS3" s="5"/>
       <c r="AT3" s="5"/>
       <c r="AU3" s="5"/>
       <c r="AV3" s="5"/>
       <c r="AW3" s="5"/>
       <c r="AX3" s="5"/>
       <c r="AY3" s="5"/>
-      <c r="AZ3" s="4">
+      <c r="AZ3" s="5"/>
+      <c r="BA3" s="4">
         <v>464</v>
       </c>
     </row>

</xml_diff>